<commit_message>
add medical records data to raw site
</commit_message>
<xml_diff>
--- a/static/data/Datasets.xlsx
+++ b/static/data/Datasets.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\website\static\data\"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Data</t>
   </si>
@@ -45,9 +45,6 @@
     <t>tab</t>
   </si>
   <si>
-    <t>Afifi Appendix A3</t>
-  </si>
-  <si>
     <t>csv</t>
   </si>
   <si>
@@ -57,18 +54,12 @@
     <t>Lung function</t>
   </si>
   <si>
-    <t>Afifi Appendix A6</t>
-  </si>
-  <si>
     <t>Chemical Companies</t>
   </si>
   <si>
     <t>fixed width</t>
   </si>
   <si>
-    <t>Afifi Ch 8.3</t>
-  </si>
-  <si>
     <t>Add Health</t>
   </si>
   <si>
@@ -121,6 +112,24 @@
   </si>
   <si>
     <t>../dm_AddHlth.html</t>
+  </si>
+  <si>
+    <t>Medical records</t>
+  </si>
+  <si>
+    <t>../medical-records.pdf</t>
+  </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>PMAS5 Appendix A6</t>
+  </si>
+  <si>
+    <t>PMAS5 Ch 8.3</t>
+  </si>
+  <si>
+    <t>PMAS5 Appendix A3</t>
   </si>
 </sst>
 </file>
@@ -961,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,99 +1008,110 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add AddHealth raw data and DM file
</commit_message>
<xml_diff>
--- a/static/data/Datasets.xlsx
+++ b/static/data/Datasets.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\website\static\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rdonatello/GitHub/website/static/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16605" windowHeight="12495"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="20900" windowHeight="12500"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -135,7 +143,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -976,17 +984,17 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1017,7 +1025,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1037,7 +1045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1054,7 +1062,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1074,7 +1082,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1094,7 +1102,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>

</xml_diff>